<commit_message>
Refactor chart config and data merge utilities
Expanded chartTypeConfig to support more chart types and modular mappings. Refactored dataMergeUtils.js to modularize data merging, filtering, and null handling, and added plugin support for filters and chart type handlers. Updated chartIcons.js to standardize GEO_MAP naming. Adjusted CSS and FileUploadModal.vue to use a more specific delete-file-btn class.
</commit_message>
<xml_diff>
--- a/test_data/sample_data.xlsx
+++ b/test_data/sample_data.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning Material\Git\Fuck-Charts\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DB598A-43CC-4BE5-90CD-6325163AE243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C157E3-8485-4F7E-8010-DDCB13CECEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="2390" windowWidth="21600" windowHeight="13210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -424,10 +435,13 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -641,7 +655,7 @@
         <v>26500</v>
       </c>
       <c r="C13">
-        <v>7300</v>
+        <v>-7300</v>
       </c>
       <c r="D13">
         <v>240</v>

</xml_diff>